<commit_message>
Auto update file on 2025-10-30 07:41
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -40,10 +40,16 @@
     <t>ZED</t>
   </si>
   <si>
+    <t>AKALI</t>
+  </si>
+  <si>
     <t>Cleaning</t>
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>test1</t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,13 +444,33 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>10000</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update file on 2025-10-30 08:44
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Linen</t>
   </si>
   <si>
     <t>test</t>
@@ -407,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,7 +453,7 @@
         <v>10000</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -470,7 +473,24 @@
         <v>200</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update file on 2025-10-30 09:31
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Linen</t>
+  </si>
+  <si>
+    <t>Utilities</t>
   </si>
   <si>
     <t>test</t>
@@ -410,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,7 +456,7 @@
         <v>10000</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -473,7 +476,7 @@
         <v>200</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -491,6 +494,23 @@
       </c>
       <c r="E4">
         <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update file on 2025-10-30 10:00
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -43,6 +43,9 @@
     <t>AKALI</t>
   </si>
   <si>
+    <t>NAMI</t>
+  </si>
+  <si>
     <t>Cleaning</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t>test1</t>
+  </si>
+  <si>
+    <t>TEST2</t>
   </si>
 </sst>
 </file>
@@ -413,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,13 +456,13 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>10000</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -470,13 +476,13 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>200</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -490,7 +496,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>200</v>
@@ -507,10 +513,30 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>500</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update expenses.xlsx from Streamlit (2025-12-04)
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2939" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="330">
   <si>
     <t>Month</t>
   </si>
@@ -1361,7 +1361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1525"/>
+  <dimension ref="A1:G1526"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -31522,6 +31522,26 @@
         <v>2025</v>
       </c>
     </row>
+    <row r="1526" spans="1:7">
+      <c r="A1526">
+        <v>11</v>
+      </c>
+      <c r="B1526" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1526">
+        <v>135</v>
+      </c>
+      <c r="E1526" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1526">
+        <v>1550</v>
+      </c>
+      <c r="G1526">
+        <v>2025</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>